<commit_message>
working on blacklist datatable
</commit_message>
<xml_diff>
--- a/public/sample_sheet_blacklist_user.xlsx
+++ b/public/sample_sheet_blacklist_user.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xamppnew\htdocs\cnkbtk\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>ip_address</t>
-  </si>
-  <si>
     <t>test23@gmail.com</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>E-mail</t>
+  </si>
+  <si>
+    <t>IP Address</t>
   </si>
 </sst>
 </file>
@@ -301,33 +301,33 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resolved bugs related to the blacklist and add one more task regading other reason field
</commit_message>
<xml_diff>
--- a/public/sample_sheet_blacklist_user.xlsx
+++ b/public/sample_sheet_blacklist_user.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>test23@gmail.com</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>IP Address</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Inappropriate content</t>
+  </si>
+  <si>
+    <t>Fraud Email</t>
   </si>
 </sst>
 </file>
@@ -298,36 +307,45 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>